<commit_message>
Update tests and files
</commit_message>
<xml_diff>
--- a/Check.xlsx
+++ b/Check.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="62">
   <si>
     <t>Группа проверок/модуль</t>
   </si>
@@ -107,9 +107,6 @@
     <t>Отображение политики конфиденциальности</t>
   </si>
   <si>
-    <t>Отображение условий использования</t>
-  </si>
-  <si>
     <t>Возврат на предыдущий экран</t>
   </si>
   <si>
@@ -135,6 +132,84 @@
   </si>
   <si>
     <t>Раскрытие текста при нажатии на стрелку</t>
+  </si>
+  <si>
+    <t>Отображение экрана авторизации</t>
+  </si>
+  <si>
+    <t>Вывод сообщения об ошибке при неверных данных</t>
+  </si>
+  <si>
+    <t>Главный экран</t>
+  </si>
+  <si>
+    <t>Нажатие кнопки "Our Mission"</t>
+  </si>
+  <si>
+    <t>Отображение заголовка News на главной странице</t>
+  </si>
+  <si>
+    <t>Успешная авторизации (отображение логотипа)</t>
+  </si>
+  <si>
+    <t>Открытие бургер-меню</t>
+  </si>
+  <si>
+    <t>Выбор пункта меню (например, "News", "About")</t>
+  </si>
+  <si>
+    <t>Видимость экрана "Our Mission"</t>
+  </si>
+  <si>
+    <t>Работоспособность стрелки для раскрытия текста</t>
+  </si>
+  <si>
+    <t>Отображения цитаты волонтера</t>
+  </si>
+  <si>
+    <t>Работоспособность кнопки Back (возврат к новостям)</t>
+  </si>
+  <si>
+    <t>Переход по ссылке Privacy Policy</t>
+  </si>
+  <si>
+    <t>Переход по ссылке Terms of Use</t>
+  </si>
+  <si>
+    <t>Кнопка переход на панель редактирования (Control Panel)</t>
+  </si>
+  <si>
+    <t>Нажатие кнопки Filter</t>
+  </si>
+  <si>
+    <t>Выбор даты ОТ</t>
+  </si>
+  <si>
+    <t>Выбор даты ДО</t>
+  </si>
+  <si>
+    <t>Выбор категории для фильтрации</t>
+  </si>
+  <si>
+    <t>Выбор статуса Active</t>
+  </si>
+  <si>
+    <t>Выбор статуса Not Active</t>
+  </si>
+  <si>
+    <t>Применение фильтров (Apply)</t>
+  </si>
+  <si>
+    <t>Сортировка новостей</t>
+  </si>
+  <si>
+    <t>Отмена создания новости</t>
+  </si>
+  <si>
+    <t>Проверка сообщения об ошибке при неверных данных</t>
+  </si>
+  <si>
+    <t>Проверка видимости панели редактирования</t>
   </si>
 </sst>
 </file>
@@ -203,7 +278,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="24">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -224,15 +299,6 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
@@ -243,19 +309,6 @@
       </top>
       <bottom style="medium">
         <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -311,34 +364,8 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -400,17 +427,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
@@ -419,17 +435,6 @@
       </right>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -488,124 +493,136 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -887,10 +904,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -902,285 +919,531 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.5" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="15" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="37"/>
+      <c r="B3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="33"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="33"/>
-      <c r="D4" s="11" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="33"/>
-      <c r="D5" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="26"/>
-      <c r="B6" s="3" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="37"/>
+      <c r="B6" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="C6" s="34"/>
-      <c r="D6" s="12" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="10" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="37"/>
+      <c r="B7" s="32" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="24"/>
+      <c r="D7" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="38"/>
+      <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="25"/>
+      <c r="D8" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="41"/>
+      <c r="B10" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="41"/>
+      <c r="B11" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="41"/>
+      <c r="B12" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="41"/>
+      <c r="D12" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="42"/>
+      <c r="B13" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="42"/>
+      <c r="D13" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C14" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="D7" s="30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="22"/>
-      <c r="B8" s="5" t="s">
+      <c r="D14" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="20"/>
+      <c r="B15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="22"/>
-      <c r="B9" s="5" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="20"/>
+      <c r="B16" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="17"/>
-      <c r="D9" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="22"/>
-      <c r="B10" s="5" t="s">
+      <c r="C16" s="22"/>
+      <c r="D16" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="20"/>
+      <c r="B17" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="17"/>
-      <c r="D10" s="35" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="23"/>
-      <c r="B11" s="5" t="s">
+      <c r="C17" s="22"/>
+      <c r="D17" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="20"/>
+      <c r="B18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C18" s="22"/>
+      <c r="D18" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A19" s="20"/>
+      <c r="B19" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="22"/>
+      <c r="D19" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="20"/>
+      <c r="B20" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="22"/>
+      <c r="D20" s="18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A21" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="15" t="s">
+      <c r="B21" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C21" s="29" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A22" s="22"/>
+      <c r="B22" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C22" s="30"/>
+      <c r="D22" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A23" s="22"/>
+      <c r="B23" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A24" s="22"/>
+      <c r="B24" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="22"/>
+      <c r="B25" s="43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C25" s="30"/>
+      <c r="D25" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="22"/>
+      <c r="B26" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="30"/>
+      <c r="D26" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="22"/>
+      <c r="B27" s="43" t="s">
+        <v>51</v>
+      </c>
+      <c r="C27" s="30"/>
+      <c r="D27" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="22"/>
+      <c r="B28" s="43" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="30"/>
+      <c r="D28" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="22"/>
+      <c r="B29" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="30"/>
+      <c r="D29" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="22"/>
+      <c r="B30" s="43" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" s="30"/>
+      <c r="D30" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="22"/>
+      <c r="B31" s="43" t="s">
+        <v>55</v>
+      </c>
+      <c r="C31" s="30"/>
+      <c r="D31" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="22"/>
+      <c r="B32" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C32" s="30"/>
+      <c r="D32" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="22"/>
+      <c r="B33" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="C33" s="30"/>
+      <c r="D33" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="22"/>
+      <c r="B34" s="43" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" s="30"/>
+      <c r="D34" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="22"/>
+      <c r="B35" s="43" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="30"/>
+      <c r="D35" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="16" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="22"/>
+      <c r="B36" s="43" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="30"/>
+      <c r="D36" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="23"/>
+      <c r="B37" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C37" s="31"/>
+      <c r="D37" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A38" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D38" s="16" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A39" s="27"/>
+      <c r="B39" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A40" s="27"/>
+      <c r="B40" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A41" s="27"/>
+      <c r="B41" s="19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A42" s="27"/>
+      <c r="B42" s="19" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="27"/>
+      <c r="D42" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A43" s="28"/>
+      <c r="B43" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" s="28"/>
+      <c r="D43" s="10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A44" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A45" s="23"/>
+      <c r="B45" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C45" s="31"/>
+      <c r="D45" s="11" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A46" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="17"/>
-      <c r="B13" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" s="19"/>
-      <c r="D13" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="17"/>
-      <c r="B14" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="17"/>
-      <c r="B15" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="16"/>
-      <c r="B16" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="36" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="37" t="s">
+      <c r="D46" s="12"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A47" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C47" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="39"/>
-      <c r="B18" s="36" t="s">
-        <v>35</v>
-      </c>
-      <c r="C18" s="39"/>
-      <c r="D18" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="38"/>
-      <c r="B19" s="36" t="s">
-        <v>36</v>
-      </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A20" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="16"/>
-      <c r="B21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D22" s="13"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A23" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="18" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" s="10"/>
-    </row>
-    <row r="24" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="16"/>
-      <c r="B24" s="6" t="s">
+      <c r="D47" s="9"/>
+    </row>
+    <row r="48" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A48" s="23"/>
+      <c r="B48" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="12"/>
+      <c r="C48" s="31"/>
+      <c r="D48" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A7:A11"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="A2:A6"/>
-    <mergeCell ref="C2:C6"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="A23:A24"/>
-    <mergeCell ref="C7:C11"/>
-    <mergeCell ref="C12:C16"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="C23:C24"/>
+  <mergeCells count="14">
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="C14:C20"/>
+    <mergeCell ref="C21:C37"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="A14:A20"/>
+    <mergeCell ref="A21:A37"/>
+    <mergeCell ref="A44:A45"/>
+    <mergeCell ref="A2:A8"/>
+    <mergeCell ref="C2:C8"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="C38:C43"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="C9:C13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>